<commit_message>
update of new KAWW ACAD script
</commit_message>
<xml_diff>
--- a/data/acad_watchlist_species.xlsx
+++ b/data/acad_watchlist_species.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylelima/Desktop/Projects/npf_project/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylelima/Desktop/Projects/npf_citsci_ms/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98004547-2E91-6E41-BB44-990FB9508838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E8A73C-F171-1A47-BA60-B11D61EAFA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14420" xr2:uid="{C070F80E-AFC0-4246-91D7-63122FEBE312}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="178">
   <si>
     <t>Achillea ptarmica</t>
   </si>
@@ -46,15 +46,9 @@
     <t>Actaea rubra</t>
   </si>
   <si>
-    <t>Agalinis paupercula</t>
-  </si>
-  <si>
     <t>Amphicarpaea bracteata</t>
   </si>
   <si>
-    <t>Andropogon gerardii</t>
-  </si>
-  <si>
     <t>Antennaria neglecta</t>
   </si>
   <si>
@@ -73,9 +67,6 @@
     <t>Atriplex glabriuscula</t>
   </si>
   <si>
-    <t>Atriplex subspicata</t>
-  </si>
-  <si>
     <t>Bartonia paniculata</t>
   </si>
   <si>
@@ -97,9 +88,6 @@
     <t>Carex ormostachya</t>
   </si>
   <si>
-    <t>Carex weigandii</t>
-  </si>
-  <si>
     <t>Centaurea nigrescens</t>
   </si>
   <si>
@@ -130,9 +118,6 @@
     <t>Cystopteris fragilis</t>
   </si>
   <si>
-    <t>Dasiphora floribunda</t>
-  </si>
-  <si>
     <t>Diphasiastrum digitatum</t>
   </si>
   <si>
@@ -187,9 +172,6 @@
     <t>Hypericum prolificum</t>
   </si>
   <si>
-    <t>Hypopitys monotropa</t>
-  </si>
-  <si>
     <t>Impatiens glandulifera</t>
   </si>
   <si>
@@ -223,9 +205,6 @@
     <t>Mertensia maritima</t>
   </si>
   <si>
-    <t>Mertensis maritima</t>
-  </si>
-  <si>
     <t>Mollugo verticillata</t>
   </si>
   <si>
@@ -301,9 +280,6 @@
     <t>Suaeda calceoliformis</t>
   </si>
   <si>
-    <t>Swida rugosa</t>
-  </si>
-  <si>
     <t>Symplocarpus foetidus</t>
   </si>
   <si>
@@ -454,9 +430,6 @@
     <t>Cardamine impatiens</t>
   </si>
   <si>
-    <t>Celastrus orbiculata</t>
-  </si>
-  <si>
     <t>Centaurea stoebe</t>
   </si>
   <si>
@@ -469,9 +442,6 @@
     <t>Euonymus spp.</t>
   </si>
   <si>
-    <t>Fallopia japonica</t>
-  </si>
-  <si>
     <t>Heracleum mantegazzianum</t>
   </si>
   <si>
@@ -499,12 +469,6 @@
     <t>Solanum dulcamara</t>
   </si>
   <si>
-    <t>Verbascum thapsis</t>
-  </si>
-  <si>
-    <t>Berberis spp.</t>
-  </si>
-  <si>
     <t>Frangula alnus</t>
   </si>
   <si>
@@ -572,6 +536,39 @@
   </si>
   <si>
     <t>Bombus terricola</t>
+  </si>
+  <si>
+    <t>Agalinis purpurea</t>
+  </si>
+  <si>
+    <t>Andropogon gerardi</t>
+  </si>
+  <si>
+    <t>Celastrus orbiculatus</t>
+  </si>
+  <si>
+    <t>Reynoutria japonica</t>
+  </si>
+  <si>
+    <t>Verbascum thapsus</t>
+  </si>
+  <si>
+    <t>Atriplex dioica</t>
+  </si>
+  <si>
+    <t>Carex wiegandii</t>
+  </si>
+  <si>
+    <t>Dasiphora fruticosa</t>
+  </si>
+  <si>
+    <t>Monotropa hypopitys</t>
+  </si>
+  <si>
+    <t>Cornus rugosa</t>
+  </si>
+  <si>
+    <t>Berberis thunbergii</t>
   </si>
 </sst>
 </file>
@@ -923,10 +920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7754563-4798-634B-89BE-DBBAAABC6080}">
-  <dimension ref="A1:C170"/>
+  <dimension ref="A1:C169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -937,13 +934,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -951,10 +948,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -962,10 +959,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -973,1836 +970,1825 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C4" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>167</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C6" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>168</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C7" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C8" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C9" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C10" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C11" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C12" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C13" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>172</v>
       </c>
       <c r="B14" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C14" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C15" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C16" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C17" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B18" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C18" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C19" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C20" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C21" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C22" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C23" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>173</v>
       </c>
       <c r="B24" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C24" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C25" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C26" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C27" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C28" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C29" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C30" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C31" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C32" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C33" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B34" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C34" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>174</v>
       </c>
       <c r="B35" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C35" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B36" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C36" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B37" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C37" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B38" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C38" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B39" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C39" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B40" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C40" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C41" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B42" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C42" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C43" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C44" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B45" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C45" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B46" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C46" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B47" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C47" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B48" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C48" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B49" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C49" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B50" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C50" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B51" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C51" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B52" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C52" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B53" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C53" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>50</v>
+        <v>175</v>
       </c>
       <c r="B54" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C54" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B55" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C55" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B56" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C56" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B57" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C57" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B58" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C58" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B59" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C59" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B60" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C60" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B61" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C61" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B62" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C62" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B63" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C63" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B64" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C64" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B65" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C65" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B66" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C66" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>163</v>
       </c>
       <c r="B67" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C67" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>175</v>
+        <v>58</v>
       </c>
       <c r="B68" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C68" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B69" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C69" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B70" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C70" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B71" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C71" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B72" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C72" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B73" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C73" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B74" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C74" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B75" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C75" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B76" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C76" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B77" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C77" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B78" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C78" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B79" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C79" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B80" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C80" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B81" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C81" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B82" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C82" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B83" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C83" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B84" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C84" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B85" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C85" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B86" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C86" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B87" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C87" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B88" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C88" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B89" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C89" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B90" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C90" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>87</v>
+        <v>176</v>
       </c>
       <c r="B91" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C91" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B92" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C92" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B93" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C93" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B94" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C94" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B95" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C95" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B96" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C96" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B97" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C97" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B98" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C98" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B99" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C99" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B100" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C100" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B101" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C101" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B102" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C102" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B103" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C103" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B104" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C104" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B105" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C105" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B106" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C106" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B107" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C107" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B108" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C108" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B109" t="s">
-        <v>111</v>
+        <v>148</v>
       </c>
       <c r="C109" t="s">
-        <v>161</v>
+        <v>105</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B110" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C110" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B111" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C111" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B112" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C112" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B113" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C113" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B114" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C114" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B115" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C115" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B116" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C116" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B117" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C117" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B118" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C118" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B119" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C119" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>124</v>
+        <v>45</v>
       </c>
       <c r="B120" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C120" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="B121" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C121" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B122" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C122" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B123" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C123" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B124" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C124" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B125" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C125" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B126" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C126" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B127" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C127" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B128" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C128" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B129" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C129" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B130" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="C130" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B131" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C131" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B132" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C132" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>137</v>
+        <v>177</v>
       </c>
       <c r="B133" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C133" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>155</v>
+        <v>130</v>
       </c>
       <c r="B134" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C134" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>138</v>
+        <v>169</v>
       </c>
       <c r="B135" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C135" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B136" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C136" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B137" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C137" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B138" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C138" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="B139" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C139" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B140" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C140" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B141" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C141" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="B142" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C142" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B143" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C143" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B144" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C144" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B145" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C145" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
+        <v>138</v>
+      </c>
+      <c r="B146" t="s">
         <v>147</v>
       </c>
-      <c r="B146" t="s">
-        <v>159</v>
-      </c>
       <c r="C146" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B147" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C147" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="B148" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C148" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>150</v>
+        <v>52</v>
       </c>
       <c r="B149" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C149" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>58</v>
+        <v>144</v>
       </c>
       <c r="B150" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C150" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="B151" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C151" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B152" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C152" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B153" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C153" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>153</v>
+        <v>90</v>
       </c>
       <c r="B154" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C154" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>98</v>
+        <v>171</v>
       </c>
       <c r="B155" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C155" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B156" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C156" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="B157" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C157" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="B158" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C158" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B159" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C159" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="B160" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C160" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B161" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C161" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B162" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C162" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B163" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C163" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B164" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C164" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="B165" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C165" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="B166" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C166" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="B167" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C167" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B168" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C168" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="B169" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="C169" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A170" t="s">
-        <v>178</v>
-      </c>
-      <c r="B170" t="s">
-        <v>176</v>
-      </c>
-      <c r="C170" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new figure version for ms
</commit_message>
<xml_diff>
--- a/data/acad_watchlist_species.xlsx
+++ b/data/acad_watchlist_species.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylelima/Desktop/Projects/npf_citsci_ms/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E8A73C-F171-1A47-BA60-B11D61EAFA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA006912-F82E-5E48-9033-724F16283E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14420" xr2:uid="{C070F80E-AFC0-4246-91D7-63122FEBE312}"/>
+    <workbookView xWindow="0" yWindow="1540" windowWidth="25600" windowHeight="14420" xr2:uid="{C070F80E-AFC0-4246-91D7-63122FEBE312}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="181">
   <si>
     <t>Achillea ptarmica</t>
   </si>
@@ -439,9 +439,6 @@
     <t>Elaeagnus umbellata</t>
   </si>
   <si>
-    <t>Euonymus spp.</t>
-  </si>
-  <si>
     <t>Heracleum mantegazzianum</t>
   </si>
   <si>
@@ -454,9 +451,6 @@
     <t>Lonicera japonica</t>
   </si>
   <si>
-    <t>Lonicera spp.</t>
-  </si>
-  <si>
     <t>Lupinus polyphyllus</t>
   </si>
   <si>
@@ -569,16 +563,37 @@
   </si>
   <si>
     <t>Berberis thunbergii</t>
+  </si>
+  <si>
+    <t>Berberis vulgaris</t>
+  </si>
+  <si>
+    <t>Euonymus alatus</t>
+  </si>
+  <si>
+    <t>Lonicera maackii</t>
+  </si>
+  <si>
+    <t>Lonicera periclymenum</t>
+  </si>
+  <si>
+    <t>Lonicera tatarica</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -604,8 +619,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -920,10 +936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7754563-4798-634B-89BE-DBBAAABC6080}">
-  <dimension ref="A1:C169"/>
+  <dimension ref="A1:C172"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A133" sqref="A133"/>
+    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="B177" sqref="B177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -951,7 +967,7 @@
         <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -962,7 +978,7 @@
         <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -973,18 +989,18 @@
         <v>103</v>
       </c>
       <c r="C4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B5" t="s">
         <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -995,18 +1011,18 @@
         <v>103</v>
       </c>
       <c r="C6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B7" t="s">
         <v>103</v>
       </c>
       <c r="C7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1017,7 +1033,7 @@
         <v>103</v>
       </c>
       <c r="C8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1028,7 +1044,7 @@
         <v>103</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1039,7 +1055,7 @@
         <v>103</v>
       </c>
       <c r="C10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1050,7 +1066,7 @@
         <v>103</v>
       </c>
       <c r="C11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1061,7 +1077,7 @@
         <v>103</v>
       </c>
       <c r="C12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1072,18 +1088,18 @@
         <v>103</v>
       </c>
       <c r="C13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B14" t="s">
         <v>103</v>
       </c>
       <c r="C14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1094,7 +1110,7 @@
         <v>103</v>
       </c>
       <c r="C15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1105,7 +1121,7 @@
         <v>103</v>
       </c>
       <c r="C16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1116,7 +1132,7 @@
         <v>103</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1127,7 +1143,7 @@
         <v>103</v>
       </c>
       <c r="C18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1138,7 +1154,7 @@
         <v>103</v>
       </c>
       <c r="C19" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1149,7 +1165,7 @@
         <v>103</v>
       </c>
       <c r="C20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1160,7 +1176,7 @@
         <v>103</v>
       </c>
       <c r="C21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1171,7 +1187,7 @@
         <v>103</v>
       </c>
       <c r="C22" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1182,18 +1198,18 @@
         <v>103</v>
       </c>
       <c r="C23" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B24" t="s">
         <v>103</v>
       </c>
       <c r="C24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -1204,7 +1220,7 @@
         <v>103</v>
       </c>
       <c r="C25" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -1215,7 +1231,7 @@
         <v>103</v>
       </c>
       <c r="C26" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -1226,7 +1242,7 @@
         <v>103</v>
       </c>
       <c r="C27" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -1237,7 +1253,7 @@
         <v>103</v>
       </c>
       <c r="C28" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -1248,7 +1264,7 @@
         <v>103</v>
       </c>
       <c r="C29" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -1259,7 +1275,7 @@
         <v>103</v>
       </c>
       <c r="C30" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -1270,7 +1286,7 @@
         <v>103</v>
       </c>
       <c r="C31" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -1281,7 +1297,7 @@
         <v>103</v>
       </c>
       <c r="C32" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1292,7 +1308,7 @@
         <v>103</v>
       </c>
       <c r="C33" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -1303,18 +1319,18 @@
         <v>103</v>
       </c>
       <c r="C34" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B35" t="s">
         <v>103</v>
       </c>
       <c r="C35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -1325,7 +1341,7 @@
         <v>103</v>
       </c>
       <c r="C36" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -1336,7 +1352,7 @@
         <v>103</v>
       </c>
       <c r="C37" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -1347,7 +1363,7 @@
         <v>103</v>
       </c>
       <c r="C38" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -1358,7 +1374,7 @@
         <v>103</v>
       </c>
       <c r="C39" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -1369,7 +1385,7 @@
         <v>103</v>
       </c>
       <c r="C40" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -1380,7 +1396,7 @@
         <v>103</v>
       </c>
       <c r="C41" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -1391,7 +1407,7 @@
         <v>103</v>
       </c>
       <c r="C42" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -1402,7 +1418,7 @@
         <v>103</v>
       </c>
       <c r="C43" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -1413,7 +1429,7 @@
         <v>103</v>
       </c>
       <c r="C44" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -1424,7 +1440,7 @@
         <v>103</v>
       </c>
       <c r="C45" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -1435,7 +1451,7 @@
         <v>103</v>
       </c>
       <c r="C46" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -1446,7 +1462,7 @@
         <v>103</v>
       </c>
       <c r="C47" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -1457,7 +1473,7 @@
         <v>103</v>
       </c>
       <c r="C48" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -1468,7 +1484,7 @@
         <v>103</v>
       </c>
       <c r="C49" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -1479,7 +1495,7 @@
         <v>103</v>
       </c>
       <c r="C50" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -1490,7 +1506,7 @@
         <v>103</v>
       </c>
       <c r="C51" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -1501,7 +1517,7 @@
         <v>103</v>
       </c>
       <c r="C52" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -1512,18 +1528,18 @@
         <v>103</v>
       </c>
       <c r="C53" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B54" t="s">
         <v>103</v>
       </c>
       <c r="C54" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -1534,7 +1550,7 @@
         <v>103</v>
       </c>
       <c r="C55" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -1545,7 +1561,7 @@
         <v>103</v>
       </c>
       <c r="C56" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -1556,7 +1572,7 @@
         <v>103</v>
       </c>
       <c r="C57" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -1567,7 +1583,7 @@
         <v>103</v>
       </c>
       <c r="C58" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -1578,7 +1594,7 @@
         <v>103</v>
       </c>
       <c r="C59" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -1589,7 +1605,7 @@
         <v>103</v>
       </c>
       <c r="C60" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -1600,7 +1616,7 @@
         <v>103</v>
       </c>
       <c r="C61" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -1611,7 +1627,7 @@
         <v>103</v>
       </c>
       <c r="C62" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -1622,7 +1638,7 @@
         <v>103</v>
       </c>
       <c r="C63" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -1633,7 +1649,7 @@
         <v>103</v>
       </c>
       <c r="C64" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -1644,7 +1660,7 @@
         <v>103</v>
       </c>
       <c r="C65" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -1655,18 +1671,18 @@
         <v>103</v>
       </c>
       <c r="C66" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B67" t="s">
         <v>103</v>
       </c>
       <c r="C67" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -1677,7 +1693,7 @@
         <v>103</v>
       </c>
       <c r="C68" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -1688,7 +1704,7 @@
         <v>103</v>
       </c>
       <c r="C69" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -1699,7 +1715,7 @@
         <v>103</v>
       </c>
       <c r="C70" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -1710,7 +1726,7 @@
         <v>103</v>
       </c>
       <c r="C71" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -1721,7 +1737,7 @@
         <v>103</v>
       </c>
       <c r="C72" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -1732,7 +1748,7 @@
         <v>103</v>
       </c>
       <c r="C73" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -1743,7 +1759,7 @@
         <v>103</v>
       </c>
       <c r="C74" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -1754,7 +1770,7 @@
         <v>103</v>
       </c>
       <c r="C75" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -1765,7 +1781,7 @@
         <v>103</v>
       </c>
       <c r="C76" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -1776,7 +1792,7 @@
         <v>103</v>
       </c>
       <c r="C77" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -1787,7 +1803,7 @@
         <v>103</v>
       </c>
       <c r="C78" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -1798,7 +1814,7 @@
         <v>103</v>
       </c>
       <c r="C79" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -1809,7 +1825,7 @@
         <v>103</v>
       </c>
       <c r="C80" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -1820,7 +1836,7 @@
         <v>103</v>
       </c>
       <c r="C81" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -1831,7 +1847,7 @@
         <v>103</v>
       </c>
       <c r="C82" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -1842,7 +1858,7 @@
         <v>103</v>
       </c>
       <c r="C83" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -1853,7 +1869,7 @@
         <v>103</v>
       </c>
       <c r="C84" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -1864,7 +1880,7 @@
         <v>103</v>
       </c>
       <c r="C85" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -1875,7 +1891,7 @@
         <v>103</v>
       </c>
       <c r="C86" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -1886,7 +1902,7 @@
         <v>103</v>
       </c>
       <c r="C87" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -1897,7 +1913,7 @@
         <v>103</v>
       </c>
       <c r="C88" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -1908,7 +1924,7 @@
         <v>103</v>
       </c>
       <c r="C89" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -1919,18 +1935,18 @@
         <v>103</v>
       </c>
       <c r="C90" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B91" t="s">
         <v>103</v>
       </c>
       <c r="C91" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -1941,7 +1957,7 @@
         <v>103</v>
       </c>
       <c r="C92" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -1952,7 +1968,7 @@
         <v>103</v>
       </c>
       <c r="C93" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -1963,7 +1979,7 @@
         <v>103</v>
       </c>
       <c r="C94" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -1974,7 +1990,7 @@
         <v>103</v>
       </c>
       <c r="C95" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -1985,7 +2001,7 @@
         <v>103</v>
       </c>
       <c r="C96" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -1996,7 +2012,7 @@
         <v>103</v>
       </c>
       <c r="C97" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -2007,7 +2023,7 @@
         <v>103</v>
       </c>
       <c r="C98" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -2018,7 +2034,7 @@
         <v>103</v>
       </c>
       <c r="C99" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -2029,7 +2045,7 @@
         <v>103</v>
       </c>
       <c r="C100" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -2040,7 +2056,7 @@
         <v>103</v>
       </c>
       <c r="C101" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -2051,7 +2067,7 @@
         <v>103</v>
       </c>
       <c r="C102" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -2062,7 +2078,7 @@
         <v>103</v>
       </c>
       <c r="C103" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -2073,7 +2089,7 @@
         <v>103</v>
       </c>
       <c r="C104" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -2084,7 +2100,7 @@
         <v>103</v>
       </c>
       <c r="C105" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -2095,7 +2111,7 @@
         <v>103</v>
       </c>
       <c r="C106" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -2106,7 +2122,7 @@
         <v>103</v>
       </c>
       <c r="C107" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -2117,7 +2133,7 @@
         <v>103</v>
       </c>
       <c r="C108" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -2125,7 +2141,7 @@
         <v>104</v>
       </c>
       <c r="B109" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C109" t="s">
         <v>105</v>
@@ -2136,7 +2152,7 @@
         <v>106</v>
       </c>
       <c r="B110" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C110" t="s">
         <v>107</v>
@@ -2147,7 +2163,7 @@
         <v>108</v>
       </c>
       <c r="B111" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C111" t="s">
         <v>107</v>
@@ -2158,7 +2174,7 @@
         <v>109</v>
       </c>
       <c r="B112" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C112" t="s">
         <v>107</v>
@@ -2169,7 +2185,7 @@
         <v>110</v>
       </c>
       <c r="B113" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C113" t="s">
         <v>107</v>
@@ -2180,7 +2196,7 @@
         <v>111</v>
       </c>
       <c r="B114" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C114" t="s">
         <v>107</v>
@@ -2191,7 +2207,7 @@
         <v>112</v>
       </c>
       <c r="B115" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C115" t="s">
         <v>107</v>
@@ -2202,7 +2218,7 @@
         <v>113</v>
       </c>
       <c r="B116" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C116" t="s">
         <v>107</v>
@@ -2213,7 +2229,7 @@
         <v>114</v>
       </c>
       <c r="B117" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C117" t="s">
         <v>107</v>
@@ -2224,18 +2240,18 @@
         <v>115</v>
       </c>
       <c r="B118" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C118" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
-        <v>116</v>
+      <c r="A119" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="B119" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C119" t="s">
         <v>107</v>
@@ -2243,21 +2259,21 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>45</v>
+        <v>179</v>
       </c>
       <c r="B120" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C120" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>117</v>
+        <v>178</v>
       </c>
       <c r="B121" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C121" t="s">
         <v>107</v>
@@ -2265,10 +2281,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B122" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C122" t="s">
         <v>107</v>
@@ -2276,10 +2292,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>119</v>
+        <v>176</v>
       </c>
       <c r="B123" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C123" t="s">
         <v>107</v>
@@ -2287,10 +2303,10 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>120</v>
+        <v>45</v>
       </c>
       <c r="B124" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C124" t="s">
         <v>107</v>
@@ -2298,10 +2314,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B125" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C125" t="s">
         <v>107</v>
@@ -2309,10 +2325,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B126" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C126" t="s">
         <v>107</v>
@@ -2320,10 +2336,10 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B127" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C127" t="s">
         <v>107</v>
@@ -2331,21 +2347,21 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B128" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C128" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B129" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C129" t="s">
         <v>107</v>
@@ -2353,32 +2369,32 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B130" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C130" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B131" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C131" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B132" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C132" t="s">
         <v>105</v>
@@ -2386,21 +2402,21 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>177</v>
+        <v>125</v>
       </c>
       <c r="B133" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C133" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B134" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C134" t="s">
         <v>105</v>
@@ -2408,10 +2424,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>169</v>
+        <v>128</v>
       </c>
       <c r="B135" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C135" t="s">
         <v>105</v>
@@ -2419,10 +2435,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B136" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C136" t="s">
         <v>105</v>
@@ -2430,10 +2446,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>146</v>
+        <v>175</v>
       </c>
       <c r="B137" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C137" t="s">
         <v>105</v>
@@ -2441,10 +2457,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
+        <v>130</v>
+      </c>
+      <c r="B138" t="s">
         <v>145</v>
-      </c>
-      <c r="B138" t="s">
-        <v>147</v>
       </c>
       <c r="C138" t="s">
         <v>105</v>
@@ -2452,10 +2468,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>132</v>
+        <v>167</v>
       </c>
       <c r="B139" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C139" t="s">
         <v>105</v>
@@ -2463,10 +2479,10 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B140" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C140" t="s">
         <v>105</v>
@@ -2474,10 +2490,10 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="B141" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C141" t="s">
         <v>105</v>
@@ -2485,10 +2501,10 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>170</v>
+        <v>143</v>
       </c>
       <c r="B142" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C142" t="s">
         <v>105</v>
@@ -2496,10 +2512,10 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B143" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C143" t="s">
         <v>105</v>
@@ -2507,10 +2523,10 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B144" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C144" t="s">
         <v>105</v>
@@ -2518,10 +2534,10 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>137</v>
+        <v>177</v>
       </c>
       <c r="B145" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C145" t="s">
         <v>105</v>
@@ -2529,10 +2545,10 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>138</v>
+        <v>168</v>
       </c>
       <c r="B146" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C146" t="s">
         <v>105</v>
@@ -2540,10 +2556,10 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B147" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C147" t="s">
         <v>105</v>
@@ -2551,10 +2567,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B148" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C148" t="s">
         <v>105</v>
@@ -2562,10 +2578,10 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>52</v>
+        <v>136</v>
       </c>
       <c r="B149" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C149" t="s">
         <v>105</v>
@@ -2573,10 +2589,10 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B150" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C150" t="s">
         <v>105</v>
@@ -2584,10 +2600,10 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B151" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C151" t="s">
         <v>105</v>
@@ -2595,10 +2611,10 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>142</v>
+        <v>52</v>
       </c>
       <c r="B152" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C152" t="s">
         <v>105</v>
@@ -2606,10 +2622,10 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B153" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C153" t="s">
         <v>105</v>
@@ -2617,10 +2633,10 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>90</v>
+        <v>139</v>
       </c>
       <c r="B154" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C154" t="s">
         <v>105</v>
@@ -2628,10 +2644,10 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
       <c r="B155" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C155" t="s">
         <v>105</v>
@@ -2639,10 +2655,10 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B156" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C156" t="s">
         <v>105</v>
@@ -2650,10 +2666,10 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>151</v>
+        <v>90</v>
       </c>
       <c r="B157" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C157" t="s">
         <v>105</v>
@@ -2661,10 +2677,10 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>152</v>
+        <v>169</v>
       </c>
       <c r="B158" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C158" t="s">
         <v>105</v>
@@ -2672,32 +2688,32 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B159" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C159" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B160" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C160" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B161" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C161" t="s">
         <v>105</v>
@@ -2705,21 +2721,21 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B162" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C162" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B163" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C163" t="s">
         <v>107</v>
@@ -2727,32 +2743,32 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B164" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C164" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B165" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C165" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B166" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C166" t="s">
         <v>107</v>
@@ -2760,34 +2776,67 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B167" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C167" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B168" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="C168" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B169" t="s">
+        <v>151</v>
+      </c>
+      <c r="C169" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>160</v>
+      </c>
+      <c r="B170" t="s">
+        <v>151</v>
+      </c>
+      <c r="C170" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>163</v>
+      </c>
+      <c r="B171" t="s">
+        <v>162</v>
+      </c>
+      <c r="C171" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
         <v>164</v>
       </c>
-      <c r="C169" t="s">
+      <c r="B172" t="s">
+        <v>162</v>
+      </c>
+      <c r="C172" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>

<commit_message>
revised analysis Jan 2025
</commit_message>
<xml_diff>
--- a/data/acad_watchlist_species.xlsx
+++ b/data/acad_watchlist_species.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylelima/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylelima/Desktop/Projects/npf_citsci_ms/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE20827-CF59-F94C-B1B5-0A9AF04CFA71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDC0026-3D68-2944-8DE7-38F71F639694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24400" windowHeight="13880" xr2:uid="{C070F80E-AFC0-4246-91D7-63122FEBE312}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{C070F80E-AFC0-4246-91D7-63122FEBE312}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="187">
   <si>
     <t>Achillea ptarmica</t>
   </si>
@@ -343,12 +343,6 @@
     <t>scientific.name</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>rare native</t>
-  </si>
-  <si>
     <t>Phellodendron amurense</t>
   </si>
   <si>
@@ -475,9 +469,6 @@
     <t>invasive not established</t>
   </si>
   <si>
-    <t>P</t>
-  </si>
-  <si>
     <t>Adelges tsugae</t>
   </si>
   <si>
@@ -520,9 +511,6 @@
     <t>Pinus resinosa</t>
   </si>
   <si>
-    <t>insect</t>
-  </si>
-  <si>
     <t>Danaus plexippus</t>
   </si>
   <si>
@@ -602,6 +590,12 @@
   </si>
   <si>
     <t>Vincetoxicum rossicum</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>species of interest</t>
   </si>
 </sst>
 </file>
@@ -652,11 +646,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -675,14 +668,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -720,7 +709,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -826,7 +815,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -968,7 +957,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -976,10 +965,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7754563-4798-634B-89BE-DBBAAABC6080}">
-  <dimension ref="A1:C182"/>
+  <dimension ref="A1:C181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" zoomScale="118" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="118" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -993,1996 +982,1989 @@
         <v>101</v>
       </c>
       <c r="B1" t="s">
-        <v>102</v>
+        <v>185</v>
       </c>
       <c r="C1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>124</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C2" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C3" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>164</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C4" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>126</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C5" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C6" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C7" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C8" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>162</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C9" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C10" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>128</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C11" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="B12" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C12" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C13" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="B14" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C14" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>130</v>
       </c>
       <c r="B15" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C15" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C16" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>172</v>
       </c>
       <c r="B17" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C17" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C18" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>139</v>
       </c>
       <c r="B19" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C19" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C20" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C21" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>131</v>
       </c>
       <c r="B22" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C22" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>170</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C23" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C24" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C25" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>132</v>
       </c>
       <c r="B26" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C26" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C27" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>133</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C28" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="B29" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C29" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C30" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>135</v>
       </c>
       <c r="B31" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C31" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C32" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>171</v>
+        <v>62</v>
       </c>
       <c r="B33" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C33" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>27</v>
+        <v>163</v>
       </c>
       <c r="B34" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C34" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>136</v>
       </c>
       <c r="B35" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C35" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>29</v>
+        <v>137</v>
       </c>
       <c r="B36" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C36" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="B37" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C37" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="B38" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C38" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
       <c r="B39" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C39" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C40" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="B41" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C41" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="B42" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C42" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>164</v>
       </c>
       <c r="B43" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="C43" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>118</v>
       </c>
       <c r="B44" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C44" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>107</v>
       </c>
       <c r="B45" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C45" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>172</v>
+        <v>108</v>
       </c>
       <c r="B46" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C46" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>109</v>
       </c>
       <c r="B47" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C47" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>116</v>
       </c>
       <c r="B48" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C48" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>104</v>
       </c>
       <c r="B49" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C49" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>111</v>
       </c>
       <c r="B50" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C50" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>171</v>
       </c>
       <c r="B51" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C51" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>110</v>
       </c>
       <c r="B52" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C52" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>106</v>
       </c>
       <c r="B53" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C53" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B54" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C54" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>114</v>
       </c>
       <c r="B55" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C55" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="B56" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C56" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>174</v>
       </c>
       <c r="B57" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C57" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>59</v>
+      <c r="A58" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="B58" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C58" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="B59" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C59" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="B60" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C60" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>113</v>
       </c>
       <c r="B61" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C61" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="B62" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C62" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="B63" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C63" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>121</v>
       </c>
       <c r="B64" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C64" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>117</v>
       </c>
       <c r="B65" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C65" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
       <c r="B66" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C66" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>69</v>
+        <v>119</v>
       </c>
       <c r="B67" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C67" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>72</v>
+        <v>183</v>
       </c>
       <c r="B68" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C68" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>73</v>
+        <v>184</v>
       </c>
       <c r="B69" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C69" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>74</v>
+        <v>176</v>
       </c>
       <c r="B70" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="C70" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>75</v>
+        <v>144</v>
       </c>
       <c r="B71" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="C71" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>76</v>
+        <v>149</v>
       </c>
       <c r="B72" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="C72" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>78</v>
+        <v>177</v>
       </c>
       <c r="B73" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="C73" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>79</v>
+        <v>178</v>
       </c>
       <c r="B74" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="C74" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>80</v>
+        <v>181</v>
       </c>
       <c r="B75" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="C75" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="B76" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="C76" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>81</v>
+        <v>180</v>
       </c>
       <c r="B77" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="C77" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>82</v>
+        <v>179</v>
       </c>
       <c r="B78" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="C78" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>83</v>
+        <v>148</v>
       </c>
       <c r="B79" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="C79" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>84</v>
+        <v>152</v>
       </c>
       <c r="B80" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="C80" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>85</v>
+        <v>153</v>
       </c>
       <c r="B81" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="C81" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>86</v>
+        <v>150</v>
       </c>
       <c r="B82" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="C82" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>88</v>
+        <v>155</v>
       </c>
       <c r="B83" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="C83" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>89</v>
+        <v>146</v>
       </c>
       <c r="B84" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="C84" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="B85" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="C85" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>92</v>
+        <v>151</v>
       </c>
       <c r="B86" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="C86" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>93</v>
+        <v>145</v>
       </c>
       <c r="B87" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="C87" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>94</v>
+        <v>154</v>
       </c>
       <c r="B88" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="C88" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="B89" t="s">
-        <v>103</v>
+        <v>186</v>
       </c>
       <c r="C89" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>95</v>
+        <v>2</v>
       </c>
       <c r="B90" t="s">
-        <v>103</v>
+        <v>186</v>
       </c>
       <c r="C90" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>96</v>
+        <v>160</v>
       </c>
       <c r="B91" t="s">
-        <v>103</v>
+        <v>186</v>
       </c>
       <c r="C91" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>97</v>
+        <v>3</v>
       </c>
       <c r="B92" t="s">
-        <v>103</v>
+        <v>186</v>
       </c>
       <c r="C92" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>104</v>
+        <v>161</v>
       </c>
       <c r="B93" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C93" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>106</v>
+        <v>4</v>
       </c>
       <c r="B94" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C94" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>187</v>
+        <v>5</v>
       </c>
       <c r="B95" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C95" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>107</v>
+      <c r="A96" t="s">
+        <v>6</v>
+      </c>
+      <c r="B96" t="s">
+        <v>186</v>
+      </c>
+      <c r="C96" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>108</v>
+        <v>7</v>
       </c>
       <c r="B97" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C97" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>109</v>
+        <v>8</v>
       </c>
       <c r="B98" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C98" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>110</v>
+        <v>165</v>
       </c>
       <c r="B99" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C99" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>111</v>
+        <v>9</v>
       </c>
       <c r="B100" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C100" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>112</v>
+        <v>10</v>
       </c>
       <c r="B101" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C101" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>113</v>
+        <v>11</v>
       </c>
       <c r="B102" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C102" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>114</v>
+        <v>159</v>
       </c>
       <c r="B103" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C103" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A104" s="1" t="s">
-        <v>179</v>
+      <c r="A104" t="s">
+        <v>99</v>
       </c>
       <c r="B104" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C104" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>178</v>
+        <v>100</v>
       </c>
       <c r="B105" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C105" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>177</v>
+        <v>13</v>
       </c>
       <c r="B106" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C106" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>115</v>
+        <v>14</v>
       </c>
       <c r="B107" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C107" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>175</v>
+        <v>15</v>
       </c>
       <c r="B108" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C108" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="B109" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C109" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>116</v>
+        <v>166</v>
       </c>
       <c r="B110" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C110" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>117</v>
+        <v>18</v>
       </c>
       <c r="B111" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C111" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>118</v>
+        <v>19</v>
       </c>
       <c r="B112" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C112" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>119</v>
+        <v>20</v>
       </c>
       <c r="B113" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C113" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>120</v>
+        <v>21</v>
       </c>
       <c r="B114" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C114" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>121</v>
+        <v>22</v>
       </c>
       <c r="B115" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C115" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>122</v>
+        <v>169</v>
       </c>
       <c r="B116" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C116" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>123</v>
+        <v>23</v>
       </c>
       <c r="B117" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C117" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>124</v>
+        <v>24</v>
       </c>
       <c r="B118" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="C118" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>126</v>
+        <v>25</v>
       </c>
       <c r="B119" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C119" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>127</v>
+        <v>26</v>
       </c>
       <c r="B120" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C120" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>0</v>
+        <v>158</v>
       </c>
       <c r="B121" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C121" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>128</v>
+        <v>167</v>
       </c>
       <c r="B122" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C122" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>174</v>
+        <v>27</v>
       </c>
       <c r="B123" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C123" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>129</v>
+        <v>28</v>
       </c>
       <c r="B124" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C124" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>166</v>
+        <v>29</v>
       </c>
       <c r="B125" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C125" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>130</v>
+        <v>30</v>
       </c>
       <c r="B126" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C126" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B127" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C127" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>143</v>
+        <v>33</v>
       </c>
       <c r="B128" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C128" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>142</v>
+        <v>35</v>
       </c>
       <c r="B129" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C129" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B130" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C130" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>131</v>
+        <v>39</v>
       </c>
       <c r="B131" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C131" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>132</v>
+        <v>40</v>
       </c>
       <c r="B132" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C132" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B133" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C133" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>176</v>
+        <v>42</v>
       </c>
       <c r="B134" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C134" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B135" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C135" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B136" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C136" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="B137" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C137" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>44</v>
-      </c>
-      <c r="B138" s="3" t="s">
-        <v>144</v>
+        <v>51</v>
+      </c>
+      <c r="B138" t="s">
+        <v>186</v>
       </c>
       <c r="C138" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B139" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C139" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B140" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C140" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>167</v>
+        <v>55</v>
       </c>
       <c r="B141" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C141" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>133</v>
+        <v>56</v>
       </c>
       <c r="B142" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C142" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="B143" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C143" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B144" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C144" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>46</v>
+        <v>157</v>
       </c>
       <c r="B145" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C145" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>135</v>
+        <v>58</v>
       </c>
       <c r="B146" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C146" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>136</v>
+        <v>59</v>
       </c>
       <c r="B147" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C147" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>137</v>
+        <v>60</v>
       </c>
       <c r="B148" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C148" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B149" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C149" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>141</v>
+        <v>63</v>
       </c>
       <c r="B150" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C150" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B151" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C151" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>138</v>
+        <v>65</v>
       </c>
       <c r="B152" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C152" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>139</v>
+        <v>66</v>
       </c>
       <c r="B153" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C153" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B154" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C154" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B155" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C155" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>140</v>
+        <v>69</v>
       </c>
       <c r="B156" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C156" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B157" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C157" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="B158" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C158" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B159" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C159" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>168</v>
+        <v>75</v>
       </c>
       <c r="B160" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C160" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>147</v>
+        <v>76</v>
       </c>
       <c r="B161" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="C161" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>180</v>
+        <v>78</v>
       </c>
       <c r="B162" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="C162" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>148</v>
+        <v>79</v>
       </c>
       <c r="B163" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="C163" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>149</v>
+        <v>80</v>
       </c>
       <c r="B164" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="C164" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>151</v>
+        <v>81</v>
       </c>
       <c r="B165" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="C165" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>152</v>
+        <v>82</v>
       </c>
       <c r="B166" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="C166" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>153</v>
+        <v>83</v>
       </c>
       <c r="B167" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="C167" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>154</v>
+        <v>84</v>
       </c>
       <c r="B168" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="C168" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>155</v>
+        <v>85</v>
       </c>
       <c r="B169" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="C169" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>156</v>
+        <v>86</v>
       </c>
       <c r="B170" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="C170" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>157</v>
+        <v>88</v>
       </c>
       <c r="B171" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="C171" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>158</v>
+        <v>89</v>
       </c>
       <c r="B172" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="C172" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>159</v>
+        <v>91</v>
       </c>
       <c r="B173" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="C173" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>181</v>
+        <v>92</v>
       </c>
       <c r="B174" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="C174" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>182</v>
+        <v>93</v>
       </c>
       <c r="B175" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="C175" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>183</v>
+        <v>94</v>
       </c>
       <c r="B176" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="C176" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>184</v>
+        <v>98</v>
       </c>
       <c r="B177" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="C177" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>186</v>
+        <v>95</v>
       </c>
       <c r="B178" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="C178" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>185</v>
+        <v>96</v>
       </c>
       <c r="B179" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="C179" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>162</v>
+        <v>97</v>
       </c>
       <c r="B180" t="s">
-        <v>161</v>
+        <v>186</v>
       </c>
       <c r="C180" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A181" t="s">
-        <v>163</v>
-      </c>
-      <c r="B181" t="s">
-        <v>161</v>
-      </c>
-      <c r="C181" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A182" s="2"/>
+      <c r="A181" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C180">
+    <sortCondition ref="B2:B180"/>
+    <sortCondition ref="A2:A180"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>